<commit_message>
Fix type issues in maintenance module outputs
</commit_message>
<xml_diff>
--- a/dds/maintenance.xlsx
+++ b/dds/maintenance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09422F9D-C1E4-4765-AB89-7000A97D54F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685CE249-B8D7-495A-9ACD-D680FBAD562B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="5">'Valid Values'!$A$1:$M$41</definedName>
     <definedName name="A">ROOT!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1925,8 +1925,8 @@
   </sheetPr>
   <dimension ref="A1:AMF93"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4545,7 +4545,7 @@
   </sheetPr>
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -5599,8 +5599,8 @@
   </sheetPr>
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7005,7 +7005,7 @@
         <v>248</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -7013,7 +7013,7 @@
         <v>251</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -7021,7 +7021,7 @@
         <v>254</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -7029,7 +7029,7 @@
         <v>257</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>